<commit_message>
updated spreadsheet and diagram. added csound6 paper
</commit_message>
<xml_diff>
--- a/icmc-2014/performancemetrics.xlsx
+++ b/icmc-2014/performancemetrics.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11000" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="8240" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -353,11 +353,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2038161560"/>
-        <c:axId val="-2132429112"/>
+        <c:axId val="2121428472"/>
+        <c:axId val="-2088110504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2038161560"/>
+        <c:axId val="2121428472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -366,7 +366,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132429112"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2088110504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -374,7 +384,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2132429112"/>
+        <c:axId val="-2088110504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -404,7 +414,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2038161560"/>
+        <c:crossAx val="2121428472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -413,6 +423,16 @@
       <c:legendPos val="t"/>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -785,7 +805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -889,7 +909,6 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Fixed mislabelling in the diagram. Lots of minor edits and improvements.
</commit_message>
<xml_diff>
--- a/icmc-2014/performancemetrics.xlsx
+++ b/icmc-2014/performancemetrics.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8240" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Minimum</t>
   </si>
@@ -44,6 +44,9 @@
   <si>
     <t>Flocking (Safari)</t>
   </si>
+  <si>
+    <t xml:space="preserve">Gibberish (Safari) </t>
+  </si>
 </sst>
 </file>
 
@@ -55,6 +58,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -172,7 +176,7 @@
                   <c:v>Flocking (Safari)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Gibberish (Chrome) </c:v>
+                  <c:v>Gibberish (Safari) </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -241,7 +245,7 @@
                   <c:v>Flocking (Safari)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Gibberish (Chrome) </c:v>
+                  <c:v>Gibberish (Safari) </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -310,7 +314,7 @@
                   <c:v>Flocking (Safari)</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Gibberish (Chrome) </c:v>
+                  <c:v>Gibberish (Safari) </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -353,11 +357,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2121428472"/>
-        <c:axId val="-2088110504"/>
+        <c:axId val="2056009720"/>
+        <c:axId val="-2113991384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2121428472"/>
+        <c:axId val="2056009720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -376,7 +380,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2088110504"/>
+        <c:crossAx val="-2113991384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -384,7 +388,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2088110504"/>
+        <c:axId val="-2113991384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -414,7 +418,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121428472"/>
+        <c:crossAx val="2056009720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -805,11 +809,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
@@ -894,7 +901,7 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>15</v>

</xml_diff>